<commit_message>
feat: melhorias nos scripts de importação
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -4,9 +4,8 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
-    <sheet name="NFs-ContasAReceber" sheetId="3" r:id="rId3"/>
-    <sheet name="Livro Caixa" sheetId="4" r:id="rId4"/>
+    <sheet name="NFs-ContasAReceber" sheetId="2" r:id="rId2"/>
+    <sheet name="Livro Caixa" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -1746,102 +1745,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Nota Fiscal</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Cliente</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Cond. Pagto</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Emissão</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Vencimento</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Valor Serviço</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Status Contas a Receber</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Cliente retém ISS?</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Alíquota ISSQN</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Alíquota Efetiva</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Valor do ISSQN</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Valor líquido</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Imp. Efetivo</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2024/124</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Hospital Manoel Gonçalves - Casa de Caridade Manoel de Sousa Moreira</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Boleto 14 dias</v>
-      </c>
-      <c r="D2" t="str">
-        <v>8/1/24</v>
-      </c>
-      <c r="E2" t="str">
-        <v>8/15/24</v>
-      </c>
-      <c r="F2" t="str">
-        <v>890</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Recebido</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Não</v>
-      </c>
-      <c r="I2" t="str">
-        <v>-</v>
-      </c>
-      <c r="J2" t="str">
-        <v>14.93</v>
-      </c>
-      <c r="K2" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="L2" t="str">
-        <v>890.00</v>
-      </c>
-      <c r="M2" t="str">
-        <v>132.89</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M220"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10874,7 +10777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2180"/>
   <sheetViews>

</xml_diff>